<commit_message>
Bug fixes and PlayerSM cleaning
+Clamp camera inversion bug fixed
+PlayerSM cleaned up
</commit_message>
<xml_diff>
--- a/Assets/1 - TODO/bugList.xlsx
+++ b/Assets/1 - TODO/bugList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityPackageProjects\FPS_PackageMaker\Assets\1 - TODO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DB9C20-9390-434F-99B0-5B73BFF90163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1241542D-B607-4863-A1E3-73EB6DAC0FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="3300" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Insufficient mask, accidental player suicide.</t>
+  </si>
+  <si>
+    <t>Camera overhaul, utilising Cinemachine</t>
+  </si>
+  <si>
+    <t>Camera overhaul. Clamp before value is set</t>
   </si>
 </sst>
 </file>
@@ -500,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,10 +554,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -568,10 +574,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added explosion ragdoll and physics
Killing the target activates its parts' rigid bodies, allowing entities to be launched when hit with lethal blow and when they are corpses
</commit_message>
<xml_diff>
--- a/Assets/1 - TODO/bugList.xlsx
+++ b/Assets/1 - TODO/bugList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityPackageProjects\FPS_PackageMaker\Assets\1 - TODO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499EC904-F5AF-4DE4-BF2E-097423AE8589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C99511A-05A4-4C47-908E-196DFD6F5B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="3300" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Bullets hit target collision, not its targets</t>
+  </si>
+  <si>
+    <t>Layer masking wasn't set to ignore the IgnoreRaycast layer fixed</t>
   </si>
 </sst>
 </file>
@@ -513,7 +516,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,10 +683,10 @@
         <v>3</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>